<commit_message>
Linking batches across conditions.
Per Chao's idea that, in the actual experiments, the KO and controls were always the same set of batches, we can now mimic this by setting "linkFlag" to 1 in the main function.
</commit_message>
<xml_diff>
--- a/Results/results_bootstrap_100k_replicates-14Oct2022.xlsx
+++ b/Results/results_bootstrap_100k_replicates-14Oct2022.xlsx
@@ -1,14 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\usr\rick\doc\Students\Kaeser, Pascal\Munc13 Paper\Munc13-Paper\Results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21450" windowHeight="5145"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" fullCalcOnLoad="true"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -57,22 +63,28 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -80,38 +92,319 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="25.4453125" customWidth="true"/>
-    <col min="2" max="2" width="6.3125" customWidth="true"/>
-    <col min="3" max="3" width="11.64453125" customWidth="true"/>
-    <col min="4" max="4" width="13.64453125" customWidth="true"/>
-    <col min="5" max="5" width="15.1796875" customWidth="true"/>
-    <col min="6" max="6" width="12.64453125" customWidth="true"/>
-    <col min="7" max="7" width="11.64453125" customWidth="true"/>
+    <col min="1" max="1" width="25.46484375" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.19921875" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -134,7 +427,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -147,8 +440,8 @@
       <c r="D2">
         <v>0.99807572899300445</v>
       </c>
-      <c r="E2">
-        <v>0.083860000000000004</v>
+      <c r="E2" s="2">
+        <v>8.3860000000000004E-2</v>
       </c>
       <c r="F2">
         <v>0.83782352879016753</v>
@@ -157,7 +450,7 @@
         <v>4.5677917131418297</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -171,7 +464,7 @@
         <v>0.42667528519679082</v>
       </c>
       <c r="E3">
-        <v>0.014590000000000001</v>
+        <v>1.4590000000000001E-2</v>
       </c>
       <c r="F3">
         <v>1.0481038742951765</v>
@@ -180,7 +473,7 @@
         <v>2.7080554961028342</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -193,8 +486,8 @@
       <c r="D4">
         <v>1.076207202566376</v>
       </c>
-      <c r="E4">
-        <v>9.0000000000000006e-05</v>
+      <c r="E4" s="2">
+        <v>9.0000000000000006E-5</v>
       </c>
       <c r="F4">
         <v>1.7135827198454561</v>
@@ -203,7 +496,7 @@
         <v>5.8636112936856808</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -217,7 +510,7 @@
         <v>0.76598806145001319</v>
       </c>
       <c r="E5">
-        <v>9.9999000009999908e-06</v>
+        <v>9.9999000009999908E-6</v>
       </c>
       <c r="F5">
         <v>2.0467655231631663</v>
@@ -226,7 +519,7 @@
         <v>5.0231620128516665</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -239,8 +532,8 @@
       <c r="D6">
         <v>0.91431014396216448</v>
       </c>
-      <c r="E6">
-        <v>0.0089700000000000005</v>
+      <c r="E6" s="2">
+        <v>8.9700000000000005E-3</v>
       </c>
       <c r="F6">
         <v>1.1609561232084311</v>
@@ -249,7 +542,7 @@
         <v>4.6790053508578175</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -263,7 +556,7 @@
         <v>0.2267212489587293</v>
       </c>
       <c r="E7">
-        <v>9.9999000009999908e-06</v>
+        <v>9.9999000009999908E-6</v>
       </c>
       <c r="F7">
         <v>1.9950326838993664</v>
@@ -272,7 +565,7 @@
         <v>2.8819476899386047</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -285,8 +578,8 @@
       <c r="D8">
         <v>0.42453802241808969</v>
       </c>
-      <c r="E8">
-        <v>0.041799999999999997</v>
+      <c r="E8" s="2">
+        <v>4.1799999999999997E-2</v>
       </c>
       <c r="F8">
         <v>0.94844125846477434</v>
@@ -295,7 +588,7 @@
         <v>2.5990656583526479</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -309,7 +602,7 @@
         <v>0.11345914562087722</v>
       </c>
       <c r="E9">
-        <v>9.9999000009999908e-06</v>
+        <v>9.9999000009999908E-6</v>
       </c>
       <c r="F9">
         <v>1.3110735779232743</v>
@@ -318,7 +611,7 @@
         <v>1.7562063158798273</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -331,7 +624,7 @@
       <c r="D10">
         <v>0.14697340107004883</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>0.30886000000000002</v>
       </c>
       <c r="F10">
@@ -341,7 +634,7 @@
         <v>1.3977270317789074</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -352,7 +645,7 @@
         <v>1.0607866654730749</v>
       </c>
       <c r="D11">
-        <v>0.068956224645870673</v>
+        <v>6.8956224645870673E-2</v>
       </c>
       <c r="E11">
         <v>0.18226000000000001</v>
@@ -364,7 +657,7 @@
         <v>1.2054989690284703</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -377,7 +670,7 @@
       <c r="D12">
         <v>0.24601685886027855</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>0.39143</v>
       </c>
       <c r="F12">
@@ -387,7 +680,7 @@
         <v>1.646266341136571</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -411,5 +704,6 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>